<commit_message>
remove config from conftest
</commit_message>
<xml_diff>
--- a/Configuration/TestData.xlsx
+++ b/Configuration/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesystems-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWright_POC/Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4E58335-8C4D-47B4-826E-0E7DA4EB8E56}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D45F353A-428B-4D5A-8415-AF48336C44C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,22 +147,22 @@
     <t>B3;P2</t>
   </si>
   <si>
+    <t>1000;rated-6009;1</t>
+  </si>
+  <si>
+    <t>500;rated-6009;1</t>
+  </si>
+  <si>
+    <t>P1;1000;P1</t>
+  </si>
+  <si>
+    <t>P2;500;P1</t>
+  </si>
+  <si>
+    <t>1000;P1</t>
+  </si>
+  <si>
     <t>500;P1</t>
-  </si>
-  <si>
-    <t>1000;rated-6009;1</t>
-  </si>
-  <si>
-    <t>500;rated-6009;1</t>
-  </si>
-  <si>
-    <t>P1;1000;P1</t>
-  </si>
-  <si>
-    <t>P2;500;P1</t>
-  </si>
-  <si>
-    <t>1000;P1</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,16 +588,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
       </c>
       <c r="P2" t="s">
         <v>13</v>
@@ -612,10 +612,10 @@
         <v>14</v>
       </c>
       <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
         <v>45</v>
-      </c>
-      <c r="X2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>